<commit_message>
tarea de lnd y pro
</commit_message>
<xml_diff>
--- a/BAE/ut03/act04/UT3.Act4-Centro educativo.xlsx
+++ b/BAE/ut03/act04/UT3.Act4-Centro educativo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="105" windowWidth="14055" windowHeight="4635" activeTab="7"/>
+    <workbookView windowHeight="16940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PROFESOR" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <sheet name="IMPARTE" sheetId="7" r:id="rId7"/>
     <sheet name="ALUMBIL" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
   <si>
     <t>DNI</t>
   </si>
@@ -35,66 +35,114 @@
     <t>SAPELLIDO</t>
   </si>
   <si>
+    <t>CIUDAD</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>ANIO</t>
+  </si>
+  <si>
+    <t>NOTA</t>
+  </si>
+  <si>
+    <t>COD_DPETO</t>
+  </si>
+  <si>
     <t>Antonio</t>
   </si>
   <si>
+    <t>Martínez</t>
+  </si>
+  <si>
+    <t>González</t>
+  </si>
+  <si>
+    <t>Sevilla</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
     <t>Dolores</t>
   </si>
   <si>
+    <t>Ramos</t>
+  </si>
+  <si>
+    <t>Cabrera</t>
+  </si>
+  <si>
+    <t>Málga</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>Ian</t>
   </si>
   <si>
+    <t>Oxley</t>
+  </si>
+  <si>
+    <t>Londres</t>
+  </si>
+  <si>
     <t>Iván</t>
   </si>
   <si>
+    <t>Sánchez</t>
+  </si>
+  <si>
+    <t>Muñoz</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
     <t>Miguel Ángel</t>
   </si>
   <si>
+    <t>Marín</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
     <t>Alejandro</t>
   </si>
   <si>
+    <t>Martín</t>
+  </si>
+  <si>
+    <t>Cantos</t>
+  </si>
+  <si>
     <t>Marta</t>
   </si>
   <si>
-    <t>Martínez</t>
-  </si>
-  <si>
-    <t>Ramos</t>
-  </si>
-  <si>
-    <t>Oxley</t>
-  </si>
-  <si>
-    <t>Sánchez</t>
-  </si>
-  <si>
-    <t>Martín</t>
-  </si>
-  <si>
     <t>Negro</t>
   </si>
   <si>
-    <t>González</t>
-  </si>
-  <si>
-    <t>Cabrera</t>
-  </si>
-  <si>
-    <t>Muñoz</t>
-  </si>
-  <si>
-    <t>Marín</t>
-  </si>
-  <si>
-    <t>Cantos</t>
-  </si>
-  <si>
     <t>Catalán</t>
   </si>
   <si>
+    <t>Bilbao</t>
+  </si>
+  <si>
     <t>CODDEP</t>
   </si>
   <si>
+    <t>JEFE_DEP</t>
+  </si>
+  <si>
+    <t>PLANTA</t>
+  </si>
+  <si>
     <t>Informática y Comunicaciones</t>
   </si>
   <si>
@@ -107,15 +155,33 @@
     <t>NUMHORAS</t>
   </si>
   <si>
+    <t>BILINGÜE</t>
+  </si>
+  <si>
+    <t>CURSO</t>
+  </si>
+  <si>
+    <t>COD_CICLO</t>
+  </si>
+  <si>
     <t>Bases de datos</t>
   </si>
   <si>
+    <t>si</t>
+  </si>
+  <si>
     <t>Lenguaje de marcas</t>
   </si>
   <si>
+    <t xml:space="preserve"> no</t>
+  </si>
+  <si>
     <t>Seguridad informática</t>
   </si>
   <si>
+    <t xml:space="preserve"> si</t>
+  </si>
+  <si>
     <t>Despliegue aplicaciones webs</t>
   </si>
   <si>
@@ -134,148 +200,91 @@
     <t>Desarrollo de aplicaciones webs</t>
   </si>
   <si>
+    <t>DAW</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>Administración de sistemas informáticos en red</t>
   </si>
   <si>
+    <t>ASIR</t>
+  </si>
+  <si>
     <t>Desarrollo de aplicaciones multiplataforma</t>
   </si>
   <si>
-    <t>DAW</t>
-  </si>
-  <si>
-    <t>ASIR</t>
-  </si>
-  <si>
     <t>DAM</t>
   </si>
   <si>
     <t>PAPELLIDO</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
     <t>Rosa</t>
   </si>
   <si>
+    <t>Blanco</t>
+  </si>
+  <si>
+    <t>Montero</t>
+  </si>
+  <si>
+    <t>García</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Pedro</t>
   </si>
   <si>
+    <t>Espinosa</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
     <t>Ángel</t>
   </si>
   <si>
+    <t>Luque</t>
+  </si>
+  <si>
+    <t>Nieto</t>
+  </si>
+  <si>
     <t>Josefa</t>
   </si>
   <si>
+    <t>Málaga</t>
+  </si>
+  <si>
     <t>Pilar</t>
   </si>
   <si>
+    <t>Cea</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
     <t>David</t>
   </si>
   <si>
-    <t>Blanco</t>
-  </si>
-  <si>
-    <t>García</t>
-  </si>
-  <si>
-    <t>Luque</t>
-  </si>
-  <si>
-    <t>Cea</t>
-  </si>
-  <si>
     <t>Chaparro</t>
   </si>
   <si>
-    <t>Montero</t>
-  </si>
-  <si>
-    <t>Espinosa</t>
-  </si>
-  <si>
-    <t>Nieto</t>
-  </si>
-  <si>
-    <t>Ruiz</t>
-  </si>
-  <si>
     <t>Gómez</t>
   </si>
   <si>
-    <t>JEFE_DEP</t>
-  </si>
-  <si>
     <t>COD_ASIG</t>
-  </si>
-  <si>
-    <t>CURSO</t>
-  </si>
-  <si>
-    <t>BILINGÜE</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>COD_CICLO</t>
-  </si>
-  <si>
-    <t>COD_DPETO</t>
-  </si>
-  <si>
-    <t>CIUDAD</t>
-  </si>
-  <si>
-    <t>Sevilla</t>
-  </si>
-  <si>
-    <t>Málga</t>
-  </si>
-  <si>
-    <t>Londres</t>
-  </si>
-  <si>
-    <t>Barcelona</t>
-  </si>
-  <si>
-    <t>Madrid</t>
-  </si>
-  <si>
-    <t>Bilbao</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>ANIO</t>
-  </si>
-  <si>
-    <t>NOTA</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>PLANTA</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Valencia</t>
-  </si>
-  <si>
-    <t>Málaga</t>
   </si>
   <si>
     <t>PF_DNI</t>
@@ -300,24 +309,367 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -325,9 +677,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -335,11 +929,63 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Énfasis6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Énfasis6" xfId="2" builtinId="51"/>
+    <cellStyle name="20% - Énfasis6" xfId="3" builtinId="50"/>
+    <cellStyle name="40% - Énfasis5" xfId="4" builtinId="47"/>
+    <cellStyle name="20% - Énfasis5" xfId="5" builtinId="46"/>
+    <cellStyle name="Énfasis5" xfId="6" builtinId="45"/>
+    <cellStyle name="40% - Énfasis4" xfId="7" builtinId="43"/>
+    <cellStyle name="Énfasis4" xfId="8" builtinId="41"/>
+    <cellStyle name="40% - Énfasis3" xfId="9" builtinId="39"/>
+    <cellStyle name="Celda vinculada" xfId="10" builtinId="24"/>
+    <cellStyle name="20% - Énfasis3" xfId="11" builtinId="38"/>
+    <cellStyle name="40% - Énfasis2" xfId="12" builtinId="35"/>
+    <cellStyle name="60% - Énfasis1" xfId="13" builtinId="32"/>
+    <cellStyle name="20% - Énfasis1" xfId="14" builtinId="30"/>
+    <cellStyle name="Moneda [0]" xfId="15" builtinId="7"/>
+    <cellStyle name="60% - Énfasis4" xfId="16" builtinId="44"/>
+    <cellStyle name="Énfasis1" xfId="17" builtinId="29"/>
+    <cellStyle name="Incorrecto" xfId="18" builtinId="27"/>
+    <cellStyle name="Correcto" xfId="19" builtinId="26"/>
+    <cellStyle name="Énfasis6" xfId="20" builtinId="49"/>
+    <cellStyle name="40% - Énfasis1" xfId="21" builtinId="31"/>
+    <cellStyle name="Total" xfId="22" builtinId="25"/>
+    <cellStyle name="60% - Énfasis2" xfId="23" builtinId="36"/>
+    <cellStyle name="Énfasis2" xfId="24" builtinId="33"/>
+    <cellStyle name="Moneda" xfId="25" builtinId="4"/>
+    <cellStyle name="Porcentaje" xfId="26" builtinId="5"/>
+    <cellStyle name="Texto explicativo" xfId="27" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="28" builtinId="16"/>
+    <cellStyle name="Celda de comprobación" xfId="29" builtinId="23"/>
+    <cellStyle name="Cálculo" xfId="30" builtinId="22"/>
+    <cellStyle name="Título 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Título 3" xfId="32" builtinId="18"/>
+    <cellStyle name="Título 2" xfId="33" builtinId="17"/>
+    <cellStyle name="20% - Énfasis2" xfId="34" builtinId="34"/>
+    <cellStyle name="Neutro" xfId="35" builtinId="28"/>
+    <cellStyle name="60% - Énfasis3" xfId="36" builtinId="40"/>
+    <cellStyle name="Título" xfId="37" builtinId="15"/>
+    <cellStyle name="Salida" xfId="38" builtinId="21"/>
+    <cellStyle name="60% - Énfasis5" xfId="39" builtinId="48"/>
+    <cellStyle name="Coma" xfId="40" builtinId="3"/>
+    <cellStyle name="Entrada" xfId="41" builtinId="20"/>
+    <cellStyle name="Nota" xfId="42" builtinId="10"/>
+    <cellStyle name="20% - Énfasis4" xfId="43" builtinId="42"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9"/>
+    <cellStyle name="Coma [0]" xfId="45" builtinId="6"/>
+    <cellStyle name="Hipervínculo" xfId="46" builtinId="8"/>
+    <cellStyle name="Énfasis3" xfId="47" builtinId="37"/>
+    <cellStyle name="Texto de advertencia" xfId="48" builtinId="11"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -622,19 +1268,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="7"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -650,19 +1296,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -670,25 +1316,25 @@
         <v>44102321</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>2013</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -699,19 +1345,19 @@
         <v>29600501</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>2019</v>
@@ -728,25 +1374,25 @@
         <v>48300100</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
       </c>
       <c r="G4">
         <v>2004</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -757,19 +1403,19 @@
         <v>84501495</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" t="s">
-        <v>76</v>
       </c>
       <c r="G5">
         <v>2018</v>
@@ -786,19 +1432,19 @@
         <v>48103100</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <v>2011</v>
@@ -815,19 +1461,19 @@
         <v>90100200</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>2019</v>
@@ -844,25 +1490,25 @@
         <v>28900194</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="G8">
         <v>2001</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -870,101 +1516,105 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
         <v>48103100</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C3">
+        <v>48300100</v>
+      </c>
+      <c r="E3">
         <v>3</v>
-      </c>
-      <c r="D3">
-        <v>48300100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -972,13 +1622,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>165</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -992,13 +1642,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1012,16 +1662,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1032,13 +1682,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1052,13 +1702,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C6">
         <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1072,13 +1722,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>180</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1089,31 +1739,33 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1121,13 +1773,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1135,13 +1787,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1149,29 +1801,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="5"/>
   <cols>
     <col min="5" max="5" width="6.140625" customWidth="1"/>
   </cols>
@@ -1184,16 +1838,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1201,19 +1855,19 @@
         <v>94342001</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1221,19 +1875,19 @@
         <v>35143098</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1241,19 +1895,19 @@
         <v>98105401</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1261,19 +1915,19 @@
         <v>13409827</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1281,19 +1935,19 @@
         <v>39099100</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1301,19 +1955,19 @@
         <v>94392805</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1321,48 +1975,50 @@
         <v>51437206</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1521,28 +2177,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1657,31 +2315,34 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>